<commit_message>
Update the email to a valid one for the combined script
</commit_message>
<xml_diff>
--- a/data/US9414_03/InputFiles/US9414_03.xlsx
+++ b/data/US9414_03/InputFiles/US9414_03.xlsx
@@ -1,20 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\huntejos\NGQ\NGQ\data\US9414_03\InputFiles\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
+  <workbookPr/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="12270" windowHeight="5340"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="145621"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -44,10 +39,10 @@
     <t>Encore CSR Group</t>
   </si>
   <si>
-    <t>jahaziel.rosales@hpe.com</t>
-  </si>
-  <si>
     <t>NI00158286</t>
+  </si>
+  <si>
+    <t>yu.li9@hpe.com</t>
   </si>
 </sst>
 </file>
@@ -376,7 +371,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -387,7 +382,7 @@
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -414,10 +409,10 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>7</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>6</v>
       </c>
       <c r="C2" t="s">
         <v>4</v>

</xml_diff>

<commit_message>
Convert: US9414_03_04_Combined_CaptureComments from ITG2 - ITG4
</commit_message>
<xml_diff>
--- a/data/US9414_03/InputFiles/US9414_03.xlsx
+++ b/data/US9414_03/InputFiles/US9414_03.xlsx
@@ -42,7 +42,7 @@
     <t>NI00158286</t>
   </si>
   <si>
-    <t>yu.li9@hpe.com</t>
+    <t>joshua.lee.hunter@hpe.com</t>
   </si>
 </sst>
 </file>
@@ -371,7 +371,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -382,7 +382,7 @@
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -425,9 +425,6 @@
       <c r="B4" s="2"/>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>